<commit_message>
Added ARFF script generator for WEKA
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/results/binary-classification-results.xlsx
+++ b/thesis-binary-classification/results/binary-classification-results.xlsx
@@ -308,15 +308,15 @@
   </sheetPr>
   <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G110" activeCellId="0" sqref="G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,23 +1385,23 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="0" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="D67" s="0" t="n">
-        <v>72.7</v>
-      </c>
-      <c r="E67" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="F67" s="0" t="n">
-        <v>2</v>
+      <c r="C67" s="1" t="n">
+        <v>0.599</v>
+      </c>
+      <c r="D67" s="1" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="E67" s="1" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="F67" s="1" t="n">
+        <v>0.483</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,22 +1485,22 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="0" t="n">
+      <c r="C73" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D73" s="0" t="n">
+      <c r="D73" s="1" t="n">
         <v>72.7</v>
       </c>
-      <c r="E73" s="0" t="n">
+      <c r="E73" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F73" s="0" t="n">
+      <c r="F73" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1585,22 +1585,22 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C79" s="0" t="n">
+      <c r="C79" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D79" s="0" t="n">
+      <c r="D79" s="1" t="n">
         <v>72.7</v>
       </c>
-      <c r="E79" s="0" t="n">
+      <c r="E79" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F79" s="0" t="n">
+      <c r="F79" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1685,22 +1685,22 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="B85" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C85" s="0" t="n">
+      <c r="C85" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D85" s="0" t="n">
+      <c r="D85" s="1" t="n">
         <v>72.7</v>
       </c>
-      <c r="E85" s="0" t="n">
+      <c r="E85" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F85" s="0" t="n">
+      <c r="F85" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1785,22 +1785,22 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+      <c r="A91" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B91" s="0" t="s">
+      <c r="B91" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C91" s="0" t="n">
+      <c r="C91" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D91" s="0" t="n">
+      <c r="D91" s="1" t="n">
         <v>72.7</v>
       </c>
-      <c r="E91" s="0" t="n">
+      <c r="E91" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F91" s="0" t="n">
+      <c r="F91" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1885,22 +1885,22 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+      <c r="A97" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B97" s="0" t="s">
+      <c r="B97" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C97" s="0" t="n">
+      <c r="C97" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D97" s="0" t="n">
+      <c r="D97" s="1" t="n">
         <v>72.7</v>
       </c>
-      <c r="E97" s="0" t="n">
+      <c r="E97" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F97" s="0" t="n">
+      <c r="F97" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1985,22 +1985,22 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
+      <c r="A103" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B103" s="0" t="s">
+      <c r="B103" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C103" s="0" t="n">
+      <c r="C103" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D103" s="0" t="n">
+      <c r="D103" s="1" t="n">
         <v>72.7</v>
       </c>
-      <c r="E103" s="0" t="n">
+      <c r="E103" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F103" s="0" t="n">
+      <c r="F103" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2085,22 +2085,22 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+      <c r="A109" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="0" t="s">
+      <c r="B109" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C109" s="0" t="n">
+      <c r="C109" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D109" s="0" t="n">
+      <c r="D109" s="1" t="n">
         <v>72.7</v>
       </c>
-      <c r="E109" s="0" t="n">
+      <c r="E109" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F109" s="0" t="n">
+      <c r="F109" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2185,22 +2185,22 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+      <c r="A115" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B115" s="0" t="s">
+      <c r="B115" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C115" s="0" t="n">
+      <c r="C115" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D115" s="0" t="n">
+      <c r="D115" s="1" t="n">
         <v>72.7</v>
       </c>
-      <c r="E115" s="0" t="n">
+      <c r="E115" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F115" s="0" t="n">
+      <c r="F115" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2285,22 +2285,22 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+      <c r="A121" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B121" s="0" t="s">
+      <c r="B121" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C121" s="0" t="n">
+      <c r="C121" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D121" s="0" t="n">
+      <c r="D121" s="1" t="n">
         <v>72.7</v>
       </c>
-      <c r="E121" s="0" t="n">
+      <c r="E121" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F121" s="0" t="n">
+      <c r="F121" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3010,14 +3010,15 @@
   </sheetPr>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B107" activeCellId="0" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5111,14 +5112,15 @@
   </sheetPr>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C105" activeCellId="0" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>